<commit_message>
Adding in bcube 15 and the final chart
</commit_message>
<xml_diff>
--- a/ntu-dsi-dcn/throughput-data/simStats.xlsx
+++ b/ntu-dsi-dcn/throughput-data/simStats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,13 +54,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,11 +88,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +191,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -194,52 +200,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Portland</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$5:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>285.727</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>253.893</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>251.021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>250.313</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fattree</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -254,23 +214,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$8</c:f>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>190.023</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>194.573</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>192.98</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>191.466</c:v>
+                  <c:v>24.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>285.727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253.893</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251.021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250.313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -278,14 +259,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$4</c:f>
+              <c:f>Sheet1!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Three Tier</c:v>
+                  <c:v>Fattree</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -300,6 +281,94 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>190.023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>194.573</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>191.466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Three Tier</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$5:$F$8</c:f>
@@ -317,6 +386,73 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>191.466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BCube</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$5:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>228.063</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>199.922</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.5287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.18419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,11 +468,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1770783968"/>
-        <c:axId val="1770785744"/>
+        <c:axId val="-1333264032"/>
+        <c:axId val="-1333261280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1770783968"/>
+        <c:axId val="-1333264032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1770785744"/>
+        <c:crossAx val="-1333261280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -387,7 +523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1770785744"/>
+        <c:axId val="-1333261280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +573,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1770783968"/>
+        <c:crossAx val="-1333264032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1565,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1616,7 +1752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1635,8 +1771,11 @@
       <c r="F5">
         <v>190.023</v>
       </c>
+      <c r="G5" s="2">
+        <v>228.06299999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1655,8 +1794,11 @@
       <c r="F6">
         <v>194.57300000000001</v>
       </c>
+      <c r="G6" s="2">
+        <v>199.922</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -1675,8 +1817,11 @@
       <c r="F7">
         <v>192.98</v>
       </c>
+      <c r="G7" s="2">
+        <v>59.528700000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>24</v>
       </c>
@@ -1694,6 +1839,9 @@
       </c>
       <c r="F8">
         <v>191.46600000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>51.184190000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>